<commit_message>
getting first maic package working
</commit_message>
<xml_diff>
--- a/data/ALD/ITC_data_extraction.xlsx
+++ b/data/ALD/ITC_data_extraction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kurttaylor/Documents/repos/maic-comparisons/data/ALD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B6F3BA-0B44-7041-8252-88FDEF152CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A153EA5-F6BA-F847-8F75-3DD46B26D683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="68800" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34560" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characteristics" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Filing name</t>
   </si>
@@ -100,19 +100,34 @@
     <t>Median Characteristic 6</t>
   </si>
   <si>
-    <t>"Intervention' characteristics taken from Scenario 22 dataset.</t>
-  </si>
-  <si>
     <t>Treatment X</t>
   </si>
   <si>
-    <t>Mean outcome Pop A</t>
-  </si>
-  <si>
-    <t>Mean outcome Pop B</t>
-  </si>
-  <si>
-    <t>"Intervention' outcomes taken from Scenario 22 dataset.</t>
+    <t>"Control' characteristics taken from Scenario 22 dataset.</t>
+  </si>
+  <si>
+    <t>"Control' outcomes taken from Scenario 22 dataset.</t>
+  </si>
+  <si>
+    <t>Mean outcome untreated</t>
+  </si>
+  <si>
+    <t>Mean outcome intervention</t>
+  </si>
+  <si>
+    <t>N patients</t>
+  </si>
+  <si>
+    <t>Untreated CI lower</t>
+  </si>
+  <si>
+    <t>Untreated CI upper</t>
+  </si>
+  <si>
+    <t>Intervention CI lower</t>
+  </si>
+  <si>
+    <t>Intervention CI upper</t>
   </si>
 </sst>
 </file>
@@ -529,12 +544,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:L17"/>
+  <dimension ref="A2:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="B17" sqref="B17"/>
+      <selection pane="topRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -598,7 +613,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -636,7 +651,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="1">
-        <v>29.52</v>
+        <v>0.24185999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -644,7 +659,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="1">
-        <v>29.66</v>
+        <v>0.25140000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -652,7 +667,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="1">
-        <v>29.95</v>
+        <v>0.25455</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -660,7 +675,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="13">
-        <v>30.77</v>
+        <v>0.24271999999999999</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -678,7 +693,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="1">
-        <v>24.89</v>
+        <v>0.25169999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -686,15 +701,23 @@
         <v>19</v>
       </c>
       <c r="B16" s="1">
-        <v>24.74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="9" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
+        <v>0.25333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="9" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>20</v>
+      <c r="B18" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -705,11 +728,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798026BB-5731-4137-BDA3-3C1FC8409E61}">
-  <dimension ref="B2:P13"/>
+  <dimension ref="B2:P17"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="134" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C11" sqref="C11"/>
+      <selection pane="topRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1288,20 +1311,58 @@
     </row>
     <row r="11" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="11">
+        <v>11.12387</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="11">
+        <v>10.541460000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="11">
+        <v>11.70628</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1">
+        <v>15.96954</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="11">
+        <v>15.185700000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1">
+        <v>16.75338</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" s="9" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" s="9" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added multi package capability to maic function - now running with maic and MAIC
</commit_message>
<xml_diff>
--- a/data/ALD/ITC_data_extraction.xlsx
+++ b/data/ALD/ITC_data_extraction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kurttaylor/Documents/repos/maic-comparisons/data/ALD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kurttaylor/Documents/Documents - Kurt’s MacBook Pro (2)/repos/maic-comparisons/data/ALD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A153EA5-F6BA-F847-8F75-3DD46B26D683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609D48F2-7B2A-E343-B6C3-A73A2BAFE5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34560" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34560" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characteristics" sheetId="1" r:id="rId1"/>
@@ -82,24 +82,6 @@
     <t>Simulation Study</t>
   </si>
   <si>
-    <t>Median Characteristic 1</t>
-  </si>
-  <si>
-    <t>Median Characteristic 2</t>
-  </si>
-  <si>
-    <t>Median Characteristic 3</t>
-  </si>
-  <si>
-    <t>Median Characteristic 4</t>
-  </si>
-  <si>
-    <t>Median Characteristic 5</t>
-  </si>
-  <si>
-    <t>Median Characteristic 6</t>
-  </si>
-  <si>
     <t>Treatment X</t>
   </si>
   <si>
@@ -128,6 +110,24 @@
   </si>
   <si>
     <t>Intervention CI upper</t>
+  </si>
+  <si>
+    <t>Mean Characteristic 1</t>
+  </si>
+  <si>
+    <t>Mean Characteristic 2</t>
+  </si>
+  <si>
+    <t>Mean Characteristic 3</t>
+  </si>
+  <si>
+    <t>Mean Characteristic 4</t>
+  </si>
+  <si>
+    <t>Mean Characteristic 5</t>
+  </si>
+  <si>
+    <t>Mean Characteristic 6</t>
   </si>
 </sst>
 </file>
@@ -546,10 +546,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="E18" sqref="E18"/>
+      <selection pane="topRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -613,7 +613,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -648,34 +648,34 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1">
-        <v>0.24185999999999999</v>
+        <v>0.24417</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1">
-        <v>0.25140000000000001</v>
+        <v>0.2487</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1">
-        <v>0.25455</v>
+        <v>0.25084000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B14" s="13">
-        <v>0.24271999999999999</v>
+        <v>0.24340000000000001</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -690,23 +690,23 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1">
-        <v>0.25169999999999998</v>
+        <v>0.2445</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1">
-        <v>0.25333</v>
+        <v>0.24737000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1">
         <v>1000</v>
@@ -717,7 +717,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -730,7 +730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798026BB-5731-4137-BDA3-3C1FC8409E61}">
   <dimension ref="B2:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="134" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="134" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C17" sqref="C17"/>
     </sheetView>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="11" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C11" s="11">
         <v>11.12387</v>
@@ -1319,7 +1319,7 @@
     </row>
     <row r="12" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C12" s="11">
         <v>10.541460000000001</v>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="13" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B13" s="10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C13" s="11">
         <v>11.70628</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="14" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1">
         <v>15.96954</v>
@@ -1343,7 +1343,7 @@
     </row>
     <row r="15" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C15" s="11">
         <v>15.185700000000001</v>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C16" s="1">
         <v>16.75338</v>
@@ -1362,7 +1362,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1992,26 +1992,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0cec425b-283a-44d8-ab13-937e9d219849">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fd6dfc79-66c6-4f79-91bd-5baad7c1fe87" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002A295D67485AEF4D8F86DD0F410C7692" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3357c116d76d89bf2059234e80923a8c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0cec425b-283a-44d8-ab13-937e9d219849" xmlns:ns3="fd6dfc79-66c6-4f79-91bd-5baad7c1fe87" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0846b1a5607fbf8c30e0c93dc2800e00" ns2:_="" ns3:_="">
     <xsd:import namespace="0cec425b-283a-44d8-ab13-937e9d219849"/>
@@ -2260,26 +2240,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{692C1CE8-9A60-4C24-91A5-348D65507C44}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0cec425b-283a-44d8-ab13-937e9d219849"/>
-    <ds:schemaRef ds:uri="fd6dfc79-66c6-4f79-91bd-5baad7c1fe87"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D921E5E-3A94-428D-8696-3B05CADBD481}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0cec425b-283a-44d8-ab13-937e9d219849">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fd6dfc79-66c6-4f79-91bd-5baad7c1fe87" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43D4D93E-1353-43CA-AAC0-0B1A9122428C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2296,4 +2277,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D921E5E-3A94-428D-8696-3B05CADBD481}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{692C1CE8-9A60-4C24-91A5-348D65507C44}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0cec425b-283a-44d8-ab13-937e9d219849"/>
+    <ds:schemaRef ds:uri="fd6dfc79-66c6-4f79-91bd-5baad7c1fe87"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding medians and proportions to the data
</commit_message>
<xml_diff>
--- a/data/ALD/ITC_data_extraction.xlsx
+++ b/data/ALD/ITC_data_extraction.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kurttaylor/Documents/Documents - Kurt’s MacBook Pro (2)/repos/maic-comparisons/data/ALD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kurttaylor/Documents/repos/maic-comparisons/data/ALD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609D48F2-7B2A-E343-B6C3-A73A2BAFE5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0DEBEA-5B35-AE4C-9A97-663040C7AE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34560" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34560" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characteristics" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Filing name</t>
   </si>
@@ -128,6 +128,36 @@
   </si>
   <si>
     <t>Mean Characteristic 6</t>
+  </si>
+  <si>
+    <t>Median Characteristic 1</t>
+  </si>
+  <si>
+    <t>Median Characteristic 2</t>
+  </si>
+  <si>
+    <t>Median Characteristic 3</t>
+  </si>
+  <si>
+    <t>Median Characteristic 4</t>
+  </si>
+  <si>
+    <t>Median Characteristic 5</t>
+  </si>
+  <si>
+    <t>Median Characteristic 6</t>
+  </si>
+  <si>
+    <t>N Characteristic 1 - No</t>
+  </si>
+  <si>
+    <t>N Characteristic 1 - Yes</t>
+  </si>
+  <si>
+    <t>N Characteristic 2 - No</t>
+  </si>
+  <si>
+    <t>N Characteristic 2 - Yes</t>
   </si>
 </sst>
 </file>
@@ -544,12 +574,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:L18"/>
+  <dimension ref="A2:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="A17" sqref="A17"/>
+      <selection pane="topRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -704,19 +734,109 @@
         <v>0.24737000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.24185999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.25140000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.25455</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="13">
+        <v>0.24271999999999999</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="13"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.25169999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.25333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="1">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="1">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="1">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="1">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B27" s="1">
         <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="9" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
+    <row r="28" spans="1:12" s="9" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B28" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1992,6 +2112,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002A295D67485AEF4D8F86DD0F410C7692" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3357c116d76d89bf2059234e80923a8c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0cec425b-283a-44d8-ab13-937e9d219849" xmlns:ns3="fd6dfc79-66c6-4f79-91bd-5baad7c1fe87" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0846b1a5607fbf8c30e0c93dc2800e00" ns2:_="" ns3:_="">
     <xsd:import namespace="0cec425b-283a-44d8-ab13-937e9d219849"/>
@@ -2240,15 +2369,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2261,6 +2381,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D921E5E-3A94-428D-8696-3B05CADBD481}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43D4D93E-1353-43CA-AAC0-0B1A9122428C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2279,14 +2407,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D921E5E-3A94-428D-8696-3B05CADBD481}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{692C1CE8-9A60-4C24-91A5-348D65507C44}">
   <ds:schemaRefs>

</xml_diff>